<commit_message>
Task 4: Long & Short Period approximation is still beeing work on
</commit_message>
<xml_diff>
--- a/Task 3/code/NT-33A_4.xlsx
+++ b/Task 3/code/NT-33A_4.xlsx
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,7 +2238,7 @@
         <v>134</v>
       </c>
       <c r="B58" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Non linear Simulator is Done & tested
</commit_message>
<xml_diff>
--- a/Task 3/code/NT-33A_4.xlsx
+++ b/Task 3/code/NT-33A_4.xlsx
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1245,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>7</v>
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
@@ -2238,7 +2238,7 @@
         <v>134</v>
       </c>
       <c r="B58" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>58</v>

</xml_diff>